<commit_message>
arruma eixo x dos gráficos de 1 ano
</commit_message>
<xml_diff>
--- a/doc/ITUB4cg_1anos.xlsx
+++ b/doc/ITUB4cg_1anos.xlsx
@@ -184,9 +184,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Retornos!$D$2:$D$250</c:f>
+              <c:f>Retornos!$D$2:$D$249</c:f>
               <c:strCache>
-                <c:ptCount val="249"/>
+                <c:ptCount val="248"/>
                 <c:pt idx="0">
                   <c:v>08/2024</c:v>
                 </c:pt>
@@ -930,19 +930,16 @@
                 </c:pt>
                 <c:pt idx="247">
                   <c:v>09/2023</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>08/2023</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retornos!$B$2:$B$250</c:f>
+              <c:f>Retornos!$B$2:$B$249</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="249"/>
+                <c:ptCount val="248"/>
                 <c:pt idx="0">
                   <c:v>0.007088331515812341</c:v>
                 </c:pt>
@@ -1686,9 +1683,6 @@
                 </c:pt>
                 <c:pt idx="247">
                   <c:v>-0.06941431670282006</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>-0.008547008547008517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1708,9 +1702,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Retornos!$D$2:$D$250</c:f>
+              <c:f>Retornos!$D$2:$D$249</c:f>
               <c:strCache>
-                <c:ptCount val="249"/>
+                <c:ptCount val="248"/>
                 <c:pt idx="0">
                   <c:v>08/2024</c:v>
                 </c:pt>
@@ -2454,19 +2448,16 @@
                 </c:pt>
                 <c:pt idx="247">
                   <c:v>09/2023</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>08/2023</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retornos!$C$2:$C$250</c:f>
+              <c:f>Retornos!$C$2:$C$249</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="249"/>
+                <c:ptCount val="248"/>
                 <c:pt idx="0">
                   <c:v>-0.009487127213420266</c:v>
                 </c:pt>
@@ -3210,9 +3201,6 @@
                 </c:pt>
                 <c:pt idx="247">
                   <c:v>0.01858443780131669</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>-0.01525503041647169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3624,6 +3612,9 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="25.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
@@ -7135,6 +7126,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="25.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">

</xml_diff>